<commit_message>
correção na chamada dos objetos de conexão da parte de migração
</commit_message>
<xml_diff>
--- a/BaseSubGrupo.xlsx
+++ b/BaseSubGrupo.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="BaseSubGrupo"/>
   </sheets>
   <definedNames>
-    <definedName name="BaseSubGrupo">'BaseSubGrupo'!$A$1:$H$788</definedName>
+    <definedName name="BaseSubGrupo">'BaseSubGrupo'!$A$1:$H$789</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -347,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H788"/>
+  <dimension ref="A1:H789"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -23458,6 +23458,38 @@
         <v>0</v>
       </c>
     </row>
+    <row outlineLevel="0" r="789">
+      <c r="A789" s="0">
+        <v>793</v>
+      </c>
+      <c r="B789" s="0" t="inlineStr">
+        <is>
+          <t>LIXA P/ LIXADEIRAS FIBRODISCO</t>
+        </is>
+      </c>
+      <c r="C789" s="0" t="inlineStr">
+        <is>
+          <t>ABRASIVO</t>
+        </is>
+      </c>
+      <c r="D789" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E789" s="1">
+        <v>0</v>
+      </c>
+      <c r="F789" s="1">
+        <v>0</v>
+      </c>
+      <c r="G789" s="1">
+        <v>0</v>
+      </c>
+      <c r="H789" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>